<commit_message>
Add starter code for resource quality/utility.
TODO: Get ReadInFile.py to work completely.
</commit_message>
<xml_diff>
--- a/input_files/countries.xlsx
+++ b/input_files/countries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boama\Desktop\Spring 2021\CS4269\CS4269_Group4_Project\input_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\CS_4269_Work\Part1\CS4269_Group4_Project\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7502DF2C-381C-4B39-AA7D-B9616EA8F440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9785117-BD25-4576-B64C-BA2BD2D29C4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22200" windowHeight="13176" xr2:uid="{8803EEA4-7768-4A59-AD8E-775F05BE9508}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8803EEA4-7768-4A59-AD8E-775F05BE9508}"/>
   </bookViews>
   <sheets>
     <sheet name="Countries" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Country</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>Erewhon</t>
+  </si>
+  <si>
+    <t>R21'</t>
+  </si>
+  <si>
+    <t>R22'</t>
+  </si>
+  <si>
+    <t>R23'</t>
   </si>
 </sst>
 </file>
@@ -423,15 +432,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDA5E0E-2D70-49FD-A817-F11261694695}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,8 +462,17 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -476,8 +494,17 @@
       <c r="G2" s="1">
         <v>0</v>
       </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -499,8 +526,17 @@
       <c r="G3" s="1">
         <v>0</v>
       </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -522,8 +558,17 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -545,8 +590,17 @@
       <c r="G5" s="1">
         <v>0</v>
       </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -568,9 +622,18 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
some addition and changes to Classes.py, ResourceQuality.py, and ReadInFile.py
</commit_message>
<xml_diff>
--- a/input_files/countries.xlsx
+++ b/input_files/countries.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\CS_4269_Work\Part1\CS4269_Group4_Project\input_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiezh\CS4269_Group4_Project\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9785117-BD25-4576-B64C-BA2BD2D29C4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E29A5F4-F407-4D3A-91B0-A739B09C7E08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8803EEA4-7768-4A59-AD8E-775F05BE9508}"/>
   </bookViews>
@@ -33,29 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Country</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>R21</t>
-  </si>
-  <si>
-    <t>R22</t>
-  </si>
-  <si>
-    <t>R23</t>
-  </si>
-  <si>
     <t>Atlantis</t>
   </si>
   <si>
@@ -71,13 +53,34 @@
     <t>Erewhon</t>
   </si>
   <si>
-    <t>R21'</t>
-  </si>
-  <si>
-    <t>R22'</t>
-  </si>
-  <si>
-    <t>R23'</t>
+    <t>population</t>
+  </si>
+  <si>
+    <t>metalElements</t>
+  </si>
+  <si>
+    <t>timber</t>
+  </si>
+  <si>
+    <t>landArea</t>
+  </si>
+  <si>
+    <t>metalAlloys</t>
+  </si>
+  <si>
+    <t>electronics</t>
+  </si>
+  <si>
+    <t>housing</t>
+  </si>
+  <si>
+    <t>metalAlloysWaste</t>
+  </si>
+  <si>
+    <t>housingWaste</t>
+  </si>
+  <si>
+    <t>electronicsWaste</t>
   </si>
 </sst>
 </file>
@@ -93,12 +96,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -113,9 +122,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -432,49 +444,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDA5E0E-2D70-49FD-A817-F11261694695}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="B2" s="1">
         <v>100</v>
@@ -486,7 +501,8 @@
         <v>2000</v>
       </c>
       <c r="E2" s="1">
-        <v>0</v>
+        <f ca="1">SUM(PRODUCT(RANDBETWEEN(0,5), 5000),10000)</f>
+        <v>20000</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -503,10 +519,13 @@
       <c r="J2" s="1">
         <v>0</v>
       </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>50</v>
@@ -518,7 +537,8 @@
         <v>1200</v>
       </c>
       <c r="E3" s="1">
-        <v>0</v>
+        <f t="shared" ref="E3:E6" ca="1" si="0">SUM(PRODUCT(RANDBETWEEN(0,5), 5000),10000)</f>
+        <v>25000</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -535,10 +555,13 @@
       <c r="J3" s="1">
         <v>0</v>
       </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>25</v>
@@ -550,7 +573,8 @@
         <v>300</v>
       </c>
       <c r="E4" s="1">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10000</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -567,10 +591,13 @@
       <c r="J4" s="1">
         <v>0</v>
       </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>30</v>
@@ -582,7 +609,8 @@
         <v>200</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>30000</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -599,10 +627,13 @@
       <c r="J5" s="1">
         <v>0</v>
       </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>70</v>
@@ -614,7 +645,8 @@
         <v>1700</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>25000</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -631,9 +663,12 @@
       <c r="J6" s="1">
         <v>0</v>
       </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changes to Classes and ReadInFile and addition of scheduler file
</commit_message>
<xml_diff>
--- a/input_files/countries.xlsx
+++ b/input_files/countries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiezh\CS4269_Group4_Project\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E29A5F4-F407-4D3A-91B0-A739B09C7E08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E6BDC7-9637-4939-97C3-4CA164464BE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8803EEA4-7768-4A59-AD8E-775F05BE9508}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Country</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>electronicsWaste</t>
+  </si>
+  <si>
+    <t>MyCountry</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -502,7 +505,7 @@
       </c>
       <c r="E2" s="1">
         <f ca="1">SUM(PRODUCT(RANDBETWEEN(0,5), 5000),10000)</f>
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -537,8 +540,8 @@
         <v>1200</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E6" ca="1" si="0">SUM(PRODUCT(RANDBETWEEN(0,5), 5000),10000)</f>
-        <v>25000</v>
+        <f t="shared" ref="E3:E7" ca="1" si="0">SUM(PRODUCT(RANDBETWEEN(0,5), 5000),10000)</f>
+        <v>30000</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -610,7 +613,7 @@
       </c>
       <c r="E5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>30000</v>
+        <v>35000</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -646,7 +649,7 @@
       </c>
       <c r="E6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>25000</v>
+        <v>15000</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -667,7 +670,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1">
+        <v>90</v>
+      </c>
+      <c r="C7" s="1">
+        <v>600</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4000</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+    </row>
     <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes to basic operators
</commit_message>
<xml_diff>
--- a/input_files/countries.xlsx
+++ b/input_files/countries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiezh\CS4269_Group4_Project\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E6BDC7-9637-4939-97C3-4CA164464BE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CEFFC5-8CB5-4AE4-A555-D59958ECAC03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8803EEA4-7768-4A59-AD8E-775F05BE9508}"/>
   </bookViews>
@@ -450,7 +450,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -505,10 +505,10 @@
       </c>
       <c r="E2" s="1">
         <f ca="1">SUM(PRODUCT(RANDBETWEEN(0,5), 5000),10000)</f>
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F2" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1">
         <v>0</v>
@@ -541,7 +541,7 @@
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E7" ca="1" si="0">SUM(PRODUCT(RANDBETWEEN(0,5), 5000),10000)</f>
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -577,7 +577,7 @@
       </c>
       <c r="E4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10000</v>
+        <v>25000</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -613,7 +613,7 @@
       </c>
       <c r="E5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>35000</v>
+        <v>30000</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -649,7 +649,7 @@
       </c>
       <c r="E6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>15000</v>
+        <v>25000</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -685,7 +685,7 @@
       </c>
       <c r="E7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>20000</v>
+        <v>25000</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Roll back faulty commit b7bdf671d4581b18c0655bd54854f7f80efd4e80 and re-apply changes.
</commit_message>
<xml_diff>
--- a/input_files/countries.xlsx
+++ b/input_files/countries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boama\Desktop\Spring 2021\CS4269\CS4269_Group4_Project\input_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiezh\CS4269_Group4_Project\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A231D45E-6044-4E7A-9B54-8EC850AA5E46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6341F25B-2F01-4597-AB9D-1B1EF6133962}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{8803EEA4-7768-4A59-AD8E-775F05BE9508}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8803EEA4-7768-4A59-AD8E-775F05BE9508}"/>
   </bookViews>
   <sheets>
     <sheet name="Countries" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Country</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>electronicsWaste</t>
+  </si>
+  <si>
+    <t>MyCountry</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>food</t>
   </si>
   <si>
     <t>foodWaste</t>
@@ -99,12 +108,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,9 +134,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -438,60 +456,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDA5E0E-2D70-49FD-A817-F11261694695}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="14.3984375" customWidth="1"/>
-    <col min="3" max="3" width="14.09765625" customWidth="1"/>
-    <col min="9" max="9" width="23.09765625" customWidth="1"/>
-    <col min="10" max="10" width="16.796875" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>16</v>
+      <c r="N1" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -505,31 +522,38 @@
         <v>2000</v>
       </c>
       <c r="E2" s="1">
-        <v>9000</v>
+        <f ca="1">SUM(PRODUCT(RANDBETWEEN(0,5), 5000),10000)</f>
+        <v>25000</v>
       </c>
       <c r="F2" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H2" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J2" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K2" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L2" s="1">
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="M2" s="1">
+        <v>100</v>
+      </c>
+      <c r="N2" s="1">
+        <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -543,31 +567,38 @@
         <v>1200</v>
       </c>
       <c r="E3" s="1">
-        <v>7000</v>
+        <f t="shared" ref="E3:E7" ca="1" si="0">SUM(PRODUCT(RANDBETWEEN(0,5), 5000),10000)</f>
+        <v>20000</v>
       </c>
       <c r="F3" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G3" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H3" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I3" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J3" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K3" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L3" s="1">
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="M3" s="1">
+        <v>100</v>
+      </c>
+      <c r="N3" s="1">
+        <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -581,31 +612,38 @@
         <v>300</v>
       </c>
       <c r="E4" s="1">
-        <v>3000</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>35000</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H4" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J4" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K4" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L4" s="1">
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="M4" s="1">
+        <v>100</v>
+      </c>
+      <c r="N4" s="1">
+        <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -619,31 +657,38 @@
         <v>200</v>
       </c>
       <c r="E5" s="1">
-        <v>1500</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10000</v>
       </c>
       <c r="F5" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G5" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J5" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K5" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L5" s="1">
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="M5" s="1">
+        <v>100</v>
+      </c>
+      <c r="N5" s="1">
+        <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -657,33 +702,85 @@
         <v>1700</v>
       </c>
       <c r="E6" s="1">
-        <v>8000</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>35000</v>
       </c>
       <c r="F6" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G6" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H6" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J6" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K6" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L6" s="1">
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="M6" s="1">
+        <v>100</v>
+      </c>
+      <c r="N6" s="1">
+        <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1">
+        <v>90</v>
+      </c>
+      <c r="C7" s="1">
+        <v>600</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4000</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="F7" s="1">
+        <v>100</v>
+      </c>
+      <c r="G7" s="1">
+        <v>100</v>
+      </c>
+      <c r="H7" s="1">
+        <v>100</v>
+      </c>
+      <c r="I7" s="1">
+        <v>100</v>
+      </c>
+      <c r="J7" s="1">
+        <v>100</v>
+      </c>
+      <c r="K7" s="1">
+        <v>100</v>
+      </c>
+      <c r="L7" s="1">
+        <v>100</v>
+      </c>
+      <c r="M7" s="1">
+        <v>100</v>
+      </c>
+      <c r="N7" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>